<commit_message>
Found travel time input data error.
Will rerun mismatching instances.
</commit_message>
<xml_diff>
--- a/12 3/ExactModelData.xlsx
+++ b/12 3/ExactModelData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\great\Google Drive\University\2020\Industrial Project 498\Exact Model Implementation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Aaron\Google Drive\University\2020\Industrial Project 498\Exact Model Implementation\12 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4A4FD1-57B6-4BCD-BD0B-9D04167F3E66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A36B59C-EAED-48A7-B874-8FD3CEFBD03C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1D" sheetId="3" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -405,40 +405,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-92.419967944089393</c:v>
+                  <c:v>6.3692648773077281</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51.269743701105639</c:v>
+                  <c:v>-42.124768164965289</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>99.463624121804799</c:v>
+                  <c:v>39.66943567681615</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-40.71152042084826</c:v>
+                  <c:v>71.251979156636224</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>71.412098282259279</c:v>
+                  <c:v>-56.142889223825691</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>82.00821554481486</c:v>
+                  <c:v>58.298406274473066</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-80.290699184430594</c:v>
+                  <c:v>-34.645480459327175</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.87095267820979</c:v>
+                  <c:v>-24.42864278558109</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-76.468914547669385</c:v>
+                  <c:v>19.113341851797983</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.4436992273353297</c:v>
+                  <c:v>-87.87552476900602</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-43.675350863631138</c:v>
+                  <c:v>21.151048954776542</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-61.732346177659053</c:v>
+                  <c:v>-90.791729618859648</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -456,40 +456,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40.695865880174992</c:v>
+                  <c:v>62.124646847679372</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-8.9945185925996043</c:v>
+                  <c:v>-91.116177049025723</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-55.23724427445508</c:v>
+                  <c:v>44.802437324990123</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>34.316995961006057</c:v>
+                  <c:v>-86.551567929601646</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-13.076866300927847</c:v>
+                  <c:v>-5.0477795188878503</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-95.813154777707894</c:v>
+                  <c:v>36.245133884398584</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.5183965217001543</c:v>
+                  <c:v>-89.322491283549226</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-61.869094939376808</c:v>
+                  <c:v>-36.452050749330411</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-32.332103862172559</c:v>
+                  <c:v>-2.1030262007637361</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-23.804359593952711</c:v>
+                  <c:v>-96.457259242617297</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-79.442711652488669</c:v>
+                  <c:v>14.508360887226686</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>50.618929914584811</c:v>
+                  <c:v>73.230788461637871</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -1558,36 +1558,36 @@
   </sheetPr>
   <dimension ref="A1:U16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.88671875" customWidth="1"/>
-    <col min="9" max="9" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" customWidth="1"/>
     <col min="15" max="15" width="24" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.44140625" customWidth="1"/>
-    <col min="21" max="21" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.44140625" customWidth="1"/>
-    <col min="23" max="23" width="5.5546875" customWidth="1"/>
-    <col min="24" max="24" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.42578125" customWidth="1"/>
+    <col min="21" max="21" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.42578125" customWidth="1"/>
+    <col min="23" max="23" width="5.5703125" customWidth="1"/>
+    <col min="24" max="24" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1650,11 +1650,11 @@
       </c>
       <c r="C2" cm="1">
         <f t="array" aca="1" ref="C2:E2" ca="1">_xlfn.XLOOKUP(B2,OFFSET($R$2,0,0,$P$8,1),OFFSET($S$2,0,0,$P$8,3))</f>
-        <v>1.4970191789459852</v>
+        <v>1.1762905920097158</v>
       </c>
       <c r="D2" s="8">
         <f ca="1"/>
-        <v>11.812562678336169</v>
+        <v>13.146694141407254</v>
       </c>
       <c r="E2" s="2">
         <f ca="1"/>
@@ -1678,9 +1678,8 @@
       <c r="K2">
         <v>24</v>
       </c>
-      <c r="L2" cm="1">
-        <f t="array" aca="1" ref="L2:L14" ca="1">_xlfn.RANDARRAY(P2+1,1,P7,P6,FALSE)</f>
-        <v>7.6181327654095604E-2</v>
+      <c r="L2">
+        <v>0</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>16</v>
@@ -1693,17 +1692,17 @@
       </c>
       <c r="S2" cm="1">
         <f t="array" aca="1" ref="S2:S4" ca="1">_xlfn.RANDARRAY(P8,1,P10,P9,FALSE)</f>
-        <v>0.87916153063992741</v>
+        <v>0.8784480500015599</v>
       </c>
       <c r="T2" cm="1">
         <f t="array" aca="1" ref="T2:T4" ca="1">_xlfn.RANDARRAY(P8,1,P12,P11,FALSE)</f>
-        <v>13.240952473869996</v>
+        <v>12.744578434295063</v>
       </c>
       <c r="U2">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1713,11 +1712,11 @@
       </c>
       <c r="C3" cm="1">
         <f t="array" aca="1" ref="C3:E3" ca="1">_xlfn.XLOOKUP(B3,OFFSET($R$2,0,0,$P$8,1),OFFSET($S$2,0,0,$P$8,3))</f>
-        <v>0.87916153063992741</v>
+        <v>0.8784480500015599</v>
       </c>
       <c r="D3" s="8">
         <f ca="1"/>
-        <v>13.240952473869996</v>
+        <v>12.744578434295063</v>
       </c>
       <c r="E3" s="2">
         <f ca="1"/>
@@ -1728,15 +1727,15 @@
       </c>
       <c r="G3" cm="1">
         <f t="array" aca="1" ref="G3:H14" ca="1">_xlfn.RANDARRAY(P2,2,P4,P3,FALSE)</f>
-        <v>-92.419967944089393</v>
+        <v>6.3692648773077281</v>
       </c>
       <c r="H3">
         <f ca="1"/>
-        <v>40.695865880174992</v>
+        <v>62.124646847679372</v>
       </c>
       <c r="I3" cm="1">
         <f t="array" aca="1" ref="I3:I14" ca="1">_xlfn.RANDARRAY(P2,1,1,ROUNDUP((P14/P2),0),TRUE)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J3">
         <f ca="1">IF(RAND()&lt;$P$5,RANDBETWEEN(5,23), 0)</f>
@@ -1746,9 +1745,9 @@
         <f ca="1">IF(J3=0,24,J3+1)</f>
         <v>24</v>
       </c>
-      <c r="L3">
-        <f ca="1"/>
-        <v>3.3930266474040433E-2</v>
+      <c r="L3" cm="1">
+        <f t="array" aca="1" ref="L3:L14" ca="1">_xlfn.RANDARRAY(P2,1,P7,P6,FALSE)</f>
+        <v>8.3449728454035782E-2</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>14</v>
@@ -1761,62 +1760,62 @@
       </c>
       <c r="S3">
         <f ca="1"/>
-        <v>1.4774115454698611</v>
+        <v>0.74561616450245838</v>
       </c>
       <c r="T3">
         <f ca="1"/>
-        <v>8.1141002188346381</v>
+        <v>13.70956953355129</v>
       </c>
       <c r="U3">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
       <c r="B4" t="str">
         <f ca="1">OFFSET($R$1,RANDBETWEEN(1,$P$8),0)</f>
-        <v>8 metre</v>
+        <v>Rigid</v>
       </c>
       <c r="C4" cm="1">
         <f t="array" aca="1" ref="C4:E4" ca="1">_xlfn.XLOOKUP(B4,OFFSET($R$2,0,0,$P$8,1),OFFSET($S$2,0,0,$P$8,3))</f>
-        <v>1.4774115454698611</v>
+        <v>0.8784480500015599</v>
       </c>
       <c r="D4" s="8">
         <f ca="1"/>
-        <v>8.1141002188346381</v>
+        <v>12.744578434295063</v>
       </c>
       <c r="E4" s="2">
         <f ca="1"/>
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4">
         <f ca="1"/>
-        <v>51.269743701105639</v>
+        <v>-42.124768164965289</v>
       </c>
       <c r="H4">
         <f ca="1"/>
-        <v>-8.9945185925996043</v>
+        <v>-91.116177049025723</v>
       </c>
       <c r="I4">
         <f ca="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J4">
         <f t="shared" ref="J4:J13" ca="1" si="0">IF(RAND()&lt;$P$5,RANDBETWEEN(5,23), 0)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <f t="shared" ref="K4:K6" ca="1" si="1">IF(J4=0,24,J4+1)</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="L4">
         <f ca="1"/>
-        <v>2.8269604744884713E-2</v>
+        <v>6.1176973653140287E-2</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>15</v>
@@ -1829,27 +1828,27 @@
       </c>
       <c r="S4">
         <f ca="1"/>
-        <v>1.4970191789459852</v>
+        <v>1.1762905920097158</v>
       </c>
       <c r="T4">
         <f ca="1"/>
-        <v>11.812562678336169</v>
+        <v>13.146694141407254</v>
       </c>
       <c r="U4">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F5">
         <v>3</v>
       </c>
       <c r="G5">
         <f ca="1"/>
-        <v>99.463624121804799</v>
+        <v>39.66943567681615</v>
       </c>
       <c r="H5">
         <f ca="1"/>
-        <v>-55.23724427445508</v>
+        <v>44.802437324990123</v>
       </c>
       <c r="I5">
         <f ca="1"/>
@@ -1865,7 +1864,7 @@
       </c>
       <c r="L5">
         <f ca="1"/>
-        <v>0.15230116846859498</v>
+        <v>0.1458423439884988</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>23</v>
@@ -1876,33 +1875,33 @@
       </c>
       <c r="R5" s="6"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F6">
         <v>4</v>
       </c>
       <c r="G6">
         <f ca="1"/>
-        <v>-40.71152042084826</v>
+        <v>71.251979156636224</v>
       </c>
       <c r="H6">
         <f ca="1"/>
-        <v>34.316995961006057</v>
+        <v>-86.551567929601646</v>
       </c>
       <c r="I6">
         <f ca="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="L6">
         <f ca="1"/>
-        <v>0.11548713918651018</v>
+        <v>9.2999964678562808E-2</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>25</v>
@@ -1913,21 +1912,21 @@
       </c>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F7">
         <v>5</v>
       </c>
       <c r="G7">
         <f ca="1"/>
-        <v>71.412098282259279</v>
+        <v>-56.142889223825691</v>
       </c>
       <c r="H7">
         <f ca="1"/>
-        <v>-13.076866300927847</v>
+        <v>-5.0477795188878503</v>
       </c>
       <c r="I7">
         <f ca="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
@@ -1939,7 +1938,7 @@
       </c>
       <c r="L7">
         <f ca="1"/>
-        <v>2.6918886181852036E-2</v>
+        <v>9.1079626510449152E-2</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>24</v>
@@ -1949,21 +1948,21 @@
         <v>1.6666666666666666E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F8">
         <v>6</v>
       </c>
       <c r="G8">
         <f ca="1"/>
-        <v>82.00821554481486</v>
+        <v>58.298406274473066</v>
       </c>
       <c r="H8">
         <f ca="1"/>
-        <v>-95.813154777707894</v>
+        <v>36.245133884398584</v>
       </c>
       <c r="I8">
         <f ca="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
@@ -1975,7 +1974,7 @@
       </c>
       <c r="L8">
         <f ca="1"/>
-        <v>0.10224312822811443</v>
+        <v>5.580902938385976E-2</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>32</v>
@@ -1984,21 +1983,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F9">
         <v>7</v>
       </c>
       <c r="G9">
         <f ca="1"/>
-        <v>-80.290699184430594</v>
+        <v>-34.645480459327175</v>
       </c>
       <c r="H9">
         <f ca="1"/>
-        <v>4.5183965217001543</v>
+        <v>-89.322491283549226</v>
       </c>
       <c r="I9">
         <f ca="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
@@ -2010,7 +2009,7 @@
       </c>
       <c r="L9">
         <f ca="1"/>
-        <v>6.9819676835636696E-2</v>
+        <v>5.7399887534259508E-2</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>20</v>
@@ -2019,17 +2018,17 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F10">
         <v>8</v>
       </c>
       <c r="G10">
         <f ca="1"/>
-        <v>12.87095267820979</v>
+        <v>-24.42864278558109</v>
       </c>
       <c r="H10">
         <f ca="1"/>
-        <v>-61.869094939376808</v>
+        <v>-36.452050749330411</v>
       </c>
       <c r="I10">
         <f ca="1"/>
@@ -2045,7 +2044,7 @@
       </c>
       <c r="L10">
         <f ca="1"/>
-        <v>2.1262248351090918E-2</v>
+        <v>0.12639559706950557</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>19</v>
@@ -2054,17 +2053,17 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F11">
         <v>9</v>
       </c>
       <c r="G11">
         <f ca="1"/>
-        <v>-76.468914547669385</v>
+        <v>19.113341851797983</v>
       </c>
       <c r="H11">
         <f ca="1"/>
-        <v>-32.332103862172559</v>
+        <v>-2.1030262007637361</v>
       </c>
       <c r="I11">
         <f ca="1"/>
@@ -2080,7 +2079,7 @@
       </c>
       <c r="L11">
         <f ca="1"/>
-        <v>6.0346996019635168E-2</v>
+        <v>2.0551140944441937E-2</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>21</v>
@@ -2089,17 +2088,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F12">
         <v>10</v>
       </c>
       <c r="G12">
         <f ca="1"/>
-        <v>7.4436992273353297</v>
+        <v>-87.87552476900602</v>
       </c>
       <c r="H12">
         <f ca="1"/>
-        <v>-23.804359593952711</v>
+        <v>-96.457259242617297</v>
       </c>
       <c r="I12">
         <f ca="1"/>
@@ -2115,7 +2114,7 @@
       </c>
       <c r="L12">
         <f ca="1"/>
-        <v>2.9141230275351399E-2</v>
+        <v>0.10204748847333264</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>22</v>
@@ -2124,21 +2123,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F13">
         <v>11</v>
       </c>
       <c r="G13">
         <f ca="1"/>
-        <v>-43.675350863631138</v>
+        <v>21.151048954776542</v>
       </c>
       <c r="H13">
         <f ca="1"/>
-        <v>-79.442711652488669</v>
+        <v>14.508360887226686</v>
       </c>
       <c r="I13">
         <f ca="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="0"/>
@@ -2150,20 +2149,20 @@
       </c>
       <c r="L13">
         <f ca="1"/>
-        <v>9.051548812262683E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+        <v>0.15897744723106896</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F14">
         <v>12</v>
       </c>
       <c r="G14">
         <f ca="1"/>
-        <v>-61.732346177659053</v>
+        <v>-90.791729618859648</v>
       </c>
       <c r="H14">
         <f ca="1"/>
-        <v>50.618929914584811</v>
+        <v>73.230788461637871</v>
       </c>
       <c r="I14">
         <f ca="1"/>
@@ -2179,17 +2178,17 @@
       </c>
       <c r="L14">
         <f ca="1"/>
-        <v>3.0376840517758769E-2</v>
+        <v>7.4654263940039434E-2</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="P14">
         <f ca="1">SUM(E:E)</f>
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
         <v>11</v>
       </c>
@@ -2216,13 +2215,13 @@
       </c>
       <c r="P15">
         <f ca="1">SUM(I:I)</f>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="P16" s="5">
         <f ca="1">P15/P14</f>
-        <v>0.6470588235294118</v>
+        <v>0.67741935483870963</v>
       </c>
     </row>
   </sheetData>
@@ -2244,70 +2243,70 @@
       <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>SQRT(('1D'!$G$2-'1D'!$G2)^2+('1D'!$H$2-'1D'!$H2)^2)</f>
         <v>0</v>
       </c>
       <c r="B1">
         <f ca="1">SQRT(('1D'!$G$3-'1D'!$G2)^2+('1D'!$H$3-'1D'!$H2)^2)</f>
-        <v>100.98318659323294</v>
+        <v>62.450294483102191</v>
       </c>
       <c r="C1">
         <f ca="1">SQRT(('1D'!$G$4-'1D'!$G2)^2+('1D'!$H$4-'1D'!$H2)^2)</f>
-        <v>52.052742328235517</v>
+        <v>100.38253739063121</v>
       </c>
       <c r="D1">
         <f ca="1">SQRT(('1D'!$G$5-'1D'!$G2)^2+('1D'!$H$5-'1D'!$H2)^2)</f>
-        <v>113.77242934243556</v>
+        <v>59.840809797133609</v>
       </c>
       <c r="E1">
         <f ca="1">SQRT(('1D'!$G$6-'1D'!$G2)^2+('1D'!$H$6-'1D'!$H2)^2)</f>
-        <v>53.24550785526278</v>
+        <v>112.10717392214546</v>
       </c>
       <c r="F1">
         <f ca="1">SQRT(('1D'!$G$7-'1D'!$G2)^2+('1D'!$H$7-'1D'!$H2)^2)</f>
-        <v>72.599533148136715</v>
+        <v>56.36935416048393</v>
       </c>
       <c r="G1">
         <f ca="1">SQRT(('1D'!$G$8-'1D'!$G2)^2+('1D'!$H$8-'1D'!$H2)^2)</f>
-        <v>126.11704105830356</v>
+        <v>68.647024002803633</v>
       </c>
       <c r="H1">
         <f ca="1">SQRT(('1D'!$G$9-'1D'!$G2)^2+('1D'!$H$9-'1D'!$H2)^2)</f>
-        <v>80.417736119913471</v>
+        <v>95.806141584750975</v>
       </c>
       <c r="I1">
         <f ca="1">SQRT(('1D'!$G$10-'1D'!$G2)^2+('1D'!$H$10-'1D'!$H2)^2)</f>
-        <v>63.193720664812389</v>
+        <v>43.880640289053247</v>
       </c>
       <c r="J1">
         <f ca="1">SQRT(('1D'!$G$11-'1D'!$G2)^2+('1D'!$H$11-'1D'!$H2)^2)</f>
-        <v>83.023248745475357</v>
+        <v>19.228690957649487</v>
       </c>
       <c r="K1">
         <f ca="1">SQRT(('1D'!$G$12-'1D'!$G2)^2+('1D'!$H$12-'1D'!$H2)^2)</f>
-        <v>24.94105438559567</v>
+        <v>130.48413970297568</v>
       </c>
       <c r="L1">
         <f ca="1">SQRT(('1D'!$G$13-'1D'!$G2)^2+('1D'!$H$13-'1D'!$H2)^2)</f>
-        <v>90.656939655835203</v>
+        <v>25.648770097635538</v>
       </c>
       <c r="M1">
         <f ca="1">SQRT(('1D'!$G$14-'1D'!$G2)^2+('1D'!$H$14-'1D'!$H2)^2)</f>
-        <v>79.832065176193368</v>
+        <v>116.64427352380943</v>
       </c>
       <c r="N1">
         <f>SQRT(('1D'!$G$15-'1D'!$G2)^2+('1D'!$H$15-'1D'!$H2)^2)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <f ca="1">SQRT(('1D'!$G$2-'1D'!$G3)^2+('1D'!$H$2-'1D'!$H3)^2)</f>
-        <v>100.98318659323294</v>
+        <v>62.450294483102191</v>
       </c>
       <c r="B2">
         <f ca="1">SQRT(('1D'!$G$3-'1D'!$G3)^2+('1D'!$H$3-'1D'!$H3)^2)</f>
@@ -2315,61 +2314,61 @@
       </c>
       <c r="C2">
         <f ca="1">SQRT(('1D'!$G$4-'1D'!$G3)^2+('1D'!$H$4-'1D'!$H3)^2)</f>
-        <v>152.03903295447341</v>
+        <v>160.7308973074127</v>
       </c>
       <c r="D2">
         <f ca="1">SQRT(('1D'!$G$5-'1D'!$G3)^2+('1D'!$H$5-'1D'!$H3)^2)</f>
-        <v>214.52849351088744</v>
+        <v>37.536120178094848</v>
       </c>
       <c r="E2">
         <f ca="1">SQRT(('1D'!$G$6-'1D'!$G3)^2+('1D'!$H$6-'1D'!$H3)^2)</f>
-        <v>52.100417721064964</v>
+        <v>162.21708742531771</v>
       </c>
       <c r="F2">
         <f ca="1">SQRT(('1D'!$G$7-'1D'!$G3)^2+('1D'!$H$7-'1D'!$H3)^2)</f>
-        <v>172.43100837788811</v>
+        <v>91.760036368430832</v>
       </c>
       <c r="G2">
         <f ca="1">SQRT(('1D'!$G$8-'1D'!$G3)^2+('1D'!$H$8-'1D'!$H3)^2)</f>
-        <v>221.49470403649192</v>
+        <v>58.020555990643601</v>
       </c>
       <c r="H2">
         <f ca="1">SQRT(('1D'!$G$9-'1D'!$G3)^2+('1D'!$H$9-'1D'!$H3)^2)</f>
-        <v>38.156630483146969</v>
+        <v>156.90266085432856</v>
       </c>
       <c r="I2">
         <f ca="1">SQRT(('1D'!$G$10-'1D'!$G3)^2+('1D'!$H$10-'1D'!$H3)^2)</f>
-        <v>146.98894228277004</v>
+        <v>103.27573008962048</v>
       </c>
       <c r="J2">
         <f ca="1">SQRT(('1D'!$G$11-'1D'!$G3)^2+('1D'!$H$11-'1D'!$H3)^2)</f>
-        <v>74.749718856626288</v>
+        <v>65.479809736661863</v>
       </c>
       <c r="K2">
         <f ca="1">SQRT(('1D'!$G$12-'1D'!$G3)^2+('1D'!$H$12-'1D'!$H3)^2)</f>
-        <v>118.88242556046039</v>
+        <v>184.47303682302626</v>
       </c>
       <c r="L2">
         <f ca="1">SQRT(('1D'!$G$13-'1D'!$G3)^2+('1D'!$H$13-'1D'!$H3)^2)</f>
-        <v>129.65074433219556</v>
+        <v>49.85791641435204</v>
       </c>
       <c r="M2">
         <f ca="1">SQRT(('1D'!$G$14-'1D'!$G3)^2+('1D'!$H$14-'1D'!$H3)^2)</f>
-        <v>32.252090312264833</v>
+        <v>97.793687081700568</v>
       </c>
       <c r="N2">
         <f ca="1">SQRT(('1D'!$G$15-'1D'!$G3)^2+('1D'!$H$15-'1D'!$H3)^2)</f>
-        <v>100.98318659323294</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+        <v>62.450294483102191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <f ca="1">SQRT(('1D'!$G$2-'1D'!$G4)^2+('1D'!$H$2-'1D'!$H4)^2)</f>
-        <v>52.052742328235517</v>
+        <v>100.38253739063121</v>
       </c>
       <c r="B3">
         <f ca="1">SQRT(('1D'!$G$3-'1D'!$G4)^2+('1D'!$H$3-'1D'!$H4)^2)</f>
-        <v>152.03903295447341</v>
+        <v>160.7308973074127</v>
       </c>
       <c r="C3">
         <f ca="1">SQRT(('1D'!$G$4-'1D'!$G4)^2+('1D'!$H$4-'1D'!$H4)^2)</f>
@@ -2377,61 +2376,61 @@
       </c>
       <c r="D3">
         <f ca="1">SQRT(('1D'!$G$5-'1D'!$G4)^2+('1D'!$H$5-'1D'!$H4)^2)</f>
-        <v>66.791015776764354</v>
+        <v>158.63215788566743</v>
       </c>
       <c r="E3">
         <f ca="1">SQRT(('1D'!$G$6-'1D'!$G4)^2+('1D'!$H$6-'1D'!$H4)^2)</f>
-        <v>101.66828533225018</v>
+        <v>113.46859693165949</v>
       </c>
       <c r="F3">
         <f ca="1">SQRT(('1D'!$G$7-'1D'!$G4)^2+('1D'!$H$7-'1D'!$H4)^2)</f>
-        <v>20.551885823072631</v>
+        <v>87.202504387355233</v>
       </c>
       <c r="G3">
         <f ca="1">SQRT(('1D'!$G$8-'1D'!$G4)^2+('1D'!$H$8-'1D'!$H4)^2)</f>
-        <v>92.099561564258821</v>
+        <v>162.19037421244903</v>
       </c>
       <c r="H3">
         <f ca="1">SQRT(('1D'!$G$9-'1D'!$G4)^2+('1D'!$H$9-'1D'!$H4)^2)</f>
-        <v>132.25259546460597</v>
+        <v>7.6913622466363174</v>
       </c>
       <c r="I3">
         <f ca="1">SQRT(('1D'!$G$10-'1D'!$G4)^2+('1D'!$H$10-'1D'!$H4)^2)</f>
-        <v>65.346675323777561</v>
+        <v>57.457110591744218</v>
       </c>
       <c r="J3">
         <f ca="1">SQRT(('1D'!$G$11-'1D'!$G4)^2+('1D'!$H$11-'1D'!$H4)^2)</f>
-        <v>129.85302344347599</v>
+        <v>108.04372791773082</v>
       </c>
       <c r="K3">
         <f ca="1">SQRT(('1D'!$G$12-'1D'!$G4)^2+('1D'!$H$12-'1D'!$H4)^2)</f>
-        <v>46.260712972264628</v>
+        <v>46.061468591881408</v>
       </c>
       <c r="L3">
         <f ca="1">SQRT(('1D'!$G$13-'1D'!$G4)^2+('1D'!$H$13-'1D'!$H4)^2)</f>
-        <v>118.22655745351892</v>
+        <v>123.12746260042005</v>
       </c>
       <c r="M3">
         <f ca="1">SQRT(('1D'!$G$14-'1D'!$G4)^2+('1D'!$H$14-'1D'!$H4)^2)</f>
-        <v>127.7624184174953</v>
+        <v>171.40127831996497</v>
       </c>
       <c r="N3">
         <f ca="1">SQRT(('1D'!$G$15-'1D'!$G4)^2+('1D'!$H$15-'1D'!$H4)^2)</f>
-        <v>52.052742328235517</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+        <v>100.38253739063121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <f ca="1">SQRT(('1D'!$G$2-'1D'!$G5)^2+('1D'!$H$2-'1D'!$H5)^2)</f>
-        <v>113.77242934243556</v>
+        <v>59.840809797133609</v>
       </c>
       <c r="B4">
         <f ca="1">SQRT(('1D'!$G$3-'1D'!$G5)^2+('1D'!$H$3-'1D'!$H5)^2)</f>
-        <v>214.52849351088744</v>
+        <v>37.536120178094848</v>
       </c>
       <c r="C4">
         <f ca="1">SQRT(('1D'!$G$4-'1D'!$G5)^2+('1D'!$H$4-'1D'!$H5)^2)</f>
-        <v>66.791015776764354</v>
+        <v>158.63215788566743</v>
       </c>
       <c r="D4">
         <f ca="1">SQRT(('1D'!$G$5-'1D'!$G5)^2+('1D'!$H$5-'1D'!$H5)^2)</f>
@@ -2439,61 +2438,61 @@
       </c>
       <c r="E4">
         <f ca="1">SQRT(('1D'!$G$6-'1D'!$G5)^2+('1D'!$H$6-'1D'!$H5)^2)</f>
-        <v>166.34011269595908</v>
+        <v>135.09748979562144</v>
       </c>
       <c r="F4">
         <f ca="1">SQRT(('1D'!$G$7-'1D'!$G5)^2+('1D'!$H$7-'1D'!$H5)^2)</f>
-        <v>50.639762764031289</v>
+        <v>108.00484119819725</v>
       </c>
       <c r="G4">
         <f ca="1">SQRT(('1D'!$G$8-'1D'!$G5)^2+('1D'!$H$8-'1D'!$H5)^2)</f>
-        <v>44.171210100671182</v>
+        <v>20.500389940260298</v>
       </c>
       <c r="H4">
         <f ca="1">SQRT(('1D'!$G$9-'1D'!$G5)^2+('1D'!$H$9-'1D'!$H5)^2)</f>
-        <v>189.42637977388929</v>
+        <v>153.33689456411915</v>
       </c>
       <c r="I4">
         <f ca="1">SQRT(('1D'!$G$10-'1D'!$G5)^2+('1D'!$H$10-'1D'!$H5)^2)</f>
-        <v>86.846256056206684</v>
+        <v>103.49326304060341</v>
       </c>
       <c r="J4">
         <f ca="1">SQRT(('1D'!$G$11-'1D'!$G5)^2+('1D'!$H$11-'1D'!$H5)^2)</f>
-        <v>177.41731488215126</v>
+        <v>51.212064027031523</v>
       </c>
       <c r="K4">
         <f ca="1">SQRT(('1D'!$G$12-'1D'!$G5)^2+('1D'!$H$12-'1D'!$H5)^2)</f>
-        <v>97.240386758391494</v>
+        <v>190.32083125474958</v>
       </c>
       <c r="L4">
         <f ca="1">SQRT(('1D'!$G$13-'1D'!$G5)^2+('1D'!$H$13-'1D'!$H5)^2)</f>
-        <v>145.17117761756396</v>
+        <v>35.505798315262069</v>
       </c>
       <c r="M4">
         <f ca="1">SQRT(('1D'!$G$14-'1D'!$G5)^2+('1D'!$H$14-'1D'!$H5)^2)</f>
-        <v>192.84623526199829</v>
+        <v>133.52260781850461</v>
       </c>
       <c r="N4">
         <f ca="1">SQRT(('1D'!$G$15-'1D'!$G5)^2+('1D'!$H$15-'1D'!$H5)^2)</f>
-        <v>113.77242934243556</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+        <v>59.840809797133609</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <f ca="1">SQRT(('1D'!$G$2-'1D'!$G6)^2+('1D'!$H$2-'1D'!$H6)^2)</f>
-        <v>53.24550785526278</v>
+        <v>112.10717392214546</v>
       </c>
       <c r="B5">
         <f ca="1">SQRT(('1D'!$G$3-'1D'!$G6)^2+('1D'!$H$3-'1D'!$H6)^2)</f>
-        <v>52.100417721064964</v>
+        <v>162.21708742531771</v>
       </c>
       <c r="C5">
         <f ca="1">SQRT(('1D'!$G$4-'1D'!$G6)^2+('1D'!$H$4-'1D'!$H6)^2)</f>
-        <v>101.66828533225018</v>
+        <v>113.46859693165949</v>
       </c>
       <c r="D5">
         <f ca="1">SQRT(('1D'!$G$5-'1D'!$G6)^2+('1D'!$H$5-'1D'!$H6)^2)</f>
-        <v>166.34011269595908</v>
+        <v>135.09748979562144</v>
       </c>
       <c r="E5">
         <f ca="1">SQRT(('1D'!$G$6-'1D'!$G6)^2+('1D'!$H$6-'1D'!$H6)^2)</f>
@@ -2501,61 +2500,61 @@
       </c>
       <c r="F5">
         <f ca="1">SQRT(('1D'!$G$7-'1D'!$G6)^2+('1D'!$H$7-'1D'!$H6)^2)</f>
-        <v>121.72873141203357</v>
+        <v>151.23597460582459</v>
       </c>
       <c r="G5">
         <f ca="1">SQRT(('1D'!$G$8-'1D'!$G6)^2+('1D'!$H$8-'1D'!$H6)^2)</f>
-        <v>178.86863818669411</v>
+        <v>123.47803459243268</v>
       </c>
       <c r="H5">
         <f ca="1">SQRT(('1D'!$G$9-'1D'!$G6)^2+('1D'!$H$9-'1D'!$H6)^2)</f>
-        <v>49.542586934311466</v>
+        <v>105.93370553958759</v>
       </c>
       <c r="I5">
         <f ca="1">SQRT(('1D'!$G$10-'1D'!$G6)^2+('1D'!$H$10-'1D'!$H6)^2)</f>
-        <v>110.10379424028945</v>
+        <v>108.00343993107724</v>
       </c>
       <c r="J5">
         <f ca="1">SQRT(('1D'!$G$11-'1D'!$G6)^2+('1D'!$H$11-'1D'!$H6)^2)</f>
-        <v>75.635267844973285</v>
+        <v>99.247134468118261</v>
       </c>
       <c r="K5">
         <f ca="1">SQRT(('1D'!$G$12-'1D'!$G6)^2+('1D'!$H$12-'1D'!$H6)^2)</f>
-        <v>75.478587366952908</v>
+        <v>159.43552059059502</v>
       </c>
       <c r="L5">
         <f ca="1">SQRT(('1D'!$G$13-'1D'!$G6)^2+('1D'!$H$13-'1D'!$H6)^2)</f>
-        <v>113.79831003666696</v>
+        <v>112.79721813747902</v>
       </c>
       <c r="M5">
         <f ca="1">SQRT(('1D'!$G$14-'1D'!$G6)^2+('1D'!$H$14-'1D'!$H6)^2)</f>
-        <v>26.601281287280955</v>
+        <v>227.57101082443432</v>
       </c>
       <c r="N5">
         <f ca="1">SQRT(('1D'!$G$15-'1D'!$G6)^2+('1D'!$H$15-'1D'!$H6)^2)</f>
-        <v>53.24550785526278</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <v>112.10717392214546</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <f ca="1">SQRT(('1D'!$G$2-'1D'!$G7)^2+('1D'!$H$2-'1D'!$H7)^2)</f>
-        <v>72.599533148136715</v>
+        <v>56.36935416048393</v>
       </c>
       <c r="B6">
         <f ca="1">SQRT(('1D'!$G$3-'1D'!$G7)^2+('1D'!$H$3-'1D'!$H7)^2)</f>
-        <v>172.43100837788811</v>
+        <v>91.760036368430832</v>
       </c>
       <c r="C6">
         <f ca="1">SQRT(('1D'!$G$4-'1D'!$G7)^2+('1D'!$H$4-'1D'!$H7)^2)</f>
-        <v>20.551885823072631</v>
+        <v>87.202504387355233</v>
       </c>
       <c r="D6">
         <f ca="1">SQRT(('1D'!$G$5-'1D'!$G7)^2+('1D'!$H$5-'1D'!$H7)^2)</f>
-        <v>50.639762764031289</v>
+        <v>108.00484119819725</v>
       </c>
       <c r="E6">
         <f ca="1">SQRT(('1D'!$G$6-'1D'!$G7)^2+('1D'!$H$6-'1D'!$H7)^2)</f>
-        <v>121.72873141203357</v>
+        <v>151.23597460582459</v>
       </c>
       <c r="F6">
         <f ca="1">SQRT(('1D'!$G$7-'1D'!$G7)^2+('1D'!$H$7-'1D'!$H7)^2)</f>
@@ -2563,61 +2562,61 @@
       </c>
       <c r="G6">
         <f ca="1">SQRT(('1D'!$G$8-'1D'!$G7)^2+('1D'!$H$8-'1D'!$H7)^2)</f>
-        <v>83.412056274586561</v>
+        <v>121.66312018298828</v>
       </c>
       <c r="H6">
         <f ca="1">SQRT(('1D'!$G$9-'1D'!$G7)^2+('1D'!$H$9-'1D'!$H7)^2)</f>
-        <v>152.71978271663721</v>
+        <v>86.973361591953491</v>
       </c>
       <c r="I6">
         <f ca="1">SQRT(('1D'!$G$10-'1D'!$G7)^2+('1D'!$H$10-'1D'!$H7)^2)</f>
-        <v>76.2085776283825</v>
+        <v>44.63207006918806</v>
       </c>
       <c r="J6">
         <f ca="1">SQRT(('1D'!$G$11-'1D'!$G7)^2+('1D'!$H$11-'1D'!$H7)^2)</f>
-        <v>149.12933356367384</v>
+        <v>75.313822687553639</v>
       </c>
       <c r="K6">
         <f ca="1">SQRT(('1D'!$G$12-'1D'!$G7)^2+('1D'!$H$12-'1D'!$H7)^2)</f>
-        <v>64.861661942952779</v>
+        <v>96.760803748243774</v>
       </c>
       <c r="L6">
         <f ca="1">SQRT(('1D'!$G$13-'1D'!$G7)^2+('1D'!$H$13-'1D'!$H7)^2)</f>
-        <v>132.85159532401258</v>
+        <v>79.729514652613119</v>
       </c>
       <c r="M6">
         <f ca="1">SQRT(('1D'!$G$14-'1D'!$G7)^2+('1D'!$H$14-'1D'!$H7)^2)</f>
-        <v>147.59606209539737</v>
+        <v>85.604184160602358</v>
       </c>
       <c r="N6">
         <f ca="1">SQRT(('1D'!$G$15-'1D'!$G7)^2+('1D'!$H$15-'1D'!$H7)^2)</f>
-        <v>72.599533148136715</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+        <v>56.36935416048393</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <f ca="1">SQRT(('1D'!$G$2-'1D'!$G8)^2+('1D'!$H$2-'1D'!$H8)^2)</f>
-        <v>126.11704105830356</v>
+        <v>68.647024002803633</v>
       </c>
       <c r="B7">
         <f ca="1">SQRT(('1D'!$G$3-'1D'!$G8)^2+('1D'!$H$3-'1D'!$H8)^2)</f>
-        <v>221.49470403649192</v>
+        <v>58.020555990643601</v>
       </c>
       <c r="C7">
         <f ca="1">SQRT(('1D'!$G$4-'1D'!$G8)^2+('1D'!$H$4-'1D'!$H8)^2)</f>
-        <v>92.099561564258821</v>
+        <v>162.19037421244903</v>
       </c>
       <c r="D7">
         <f ca="1">SQRT(('1D'!$G$5-'1D'!$G8)^2+('1D'!$H$5-'1D'!$H8)^2)</f>
-        <v>44.171210100671182</v>
+        <v>20.500389940260298</v>
       </c>
       <c r="E7">
         <f ca="1">SQRT(('1D'!$G$6-'1D'!$G8)^2+('1D'!$H$6-'1D'!$H8)^2)</f>
-        <v>178.86863818669411</v>
+        <v>123.47803459243268</v>
       </c>
       <c r="F7">
         <f ca="1">SQRT(('1D'!$G$7-'1D'!$G8)^2+('1D'!$H$7-'1D'!$H8)^2)</f>
-        <v>83.412056274586561</v>
+        <v>121.66312018298828</v>
       </c>
       <c r="G7">
         <f ca="1">SQRT(('1D'!$G$8-'1D'!$G8)^2+('1D'!$H$8-'1D'!$H8)^2)</f>
@@ -2625,61 +2624,61 @@
       </c>
       <c r="H7">
         <f ca="1">SQRT(('1D'!$G$9-'1D'!$G8)^2+('1D'!$H$9-'1D'!$H8)^2)</f>
-        <v>190.80712226863187</v>
+        <v>156.2235403884566</v>
       </c>
       <c r="I7">
         <f ca="1">SQRT(('1D'!$G$10-'1D'!$G8)^2+('1D'!$H$10-'1D'!$H8)^2)</f>
-        <v>77.020518792035219</v>
+        <v>110.13012893779381</v>
       </c>
       <c r="J7">
         <f ca="1">SQRT(('1D'!$G$11-'1D'!$G8)^2+('1D'!$H$11-'1D'!$H8)^2)</f>
-        <v>170.71861230601354</v>
+        <v>54.827462605216674</v>
       </c>
       <c r="K7">
         <f ca="1">SQRT(('1D'!$G$12-'1D'!$G8)^2+('1D'!$H$12-'1D'!$H8)^2)</f>
-        <v>103.65873661913729</v>
+        <v>197.42528525581736</v>
       </c>
       <c r="L7">
         <f ca="1">SQRT(('1D'!$G$13-'1D'!$G8)^2+('1D'!$H$13-'1D'!$H8)^2)</f>
-        <v>126.74521795027334</v>
+        <v>43.039673049034562</v>
       </c>
       <c r="M7">
         <f ca="1">SQRT(('1D'!$G$14-'1D'!$G8)^2+('1D'!$H$14-'1D'!$H8)^2)</f>
-        <v>205.1918724307157</v>
+        <v>153.60926816178537</v>
       </c>
       <c r="N7">
         <f ca="1">SQRT(('1D'!$G$15-'1D'!$G8)^2+('1D'!$H$15-'1D'!$H8)^2)</f>
-        <v>126.11704105830356</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+        <v>68.647024002803633</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <f ca="1">SQRT(('1D'!$G$2-'1D'!$G9)^2+('1D'!$H$2-'1D'!$H9)^2)</f>
-        <v>80.417736119913471</v>
+        <v>95.806141584750975</v>
       </c>
       <c r="B8">
         <f ca="1">SQRT(('1D'!$G$3-'1D'!$G9)^2+('1D'!$H$3-'1D'!$H9)^2)</f>
-        <v>38.156630483146969</v>
+        <v>156.90266085432856</v>
       </c>
       <c r="C8">
         <f ca="1">SQRT(('1D'!$G$4-'1D'!$G9)^2+('1D'!$H$4-'1D'!$H9)^2)</f>
-        <v>132.25259546460597</v>
+        <v>7.6913622466363174</v>
       </c>
       <c r="D8">
         <f ca="1">SQRT(('1D'!$G$5-'1D'!$G9)^2+('1D'!$H$5-'1D'!$H9)^2)</f>
-        <v>189.42637977388929</v>
+        <v>153.33689456411915</v>
       </c>
       <c r="E8">
         <f ca="1">SQRT(('1D'!$G$6-'1D'!$G9)^2+('1D'!$H$6-'1D'!$H9)^2)</f>
-        <v>49.542586934311466</v>
+        <v>105.93370553958759</v>
       </c>
       <c r="F8">
         <f ca="1">SQRT(('1D'!$G$7-'1D'!$G9)^2+('1D'!$H$7-'1D'!$H9)^2)</f>
-        <v>152.71978271663721</v>
+        <v>86.973361591953491</v>
       </c>
       <c r="G8">
         <f ca="1">SQRT(('1D'!$G$8-'1D'!$G9)^2+('1D'!$H$8-'1D'!$H9)^2)</f>
-        <v>190.80712226863187</v>
+        <v>156.2235403884566</v>
       </c>
       <c r="H8">
         <f ca="1">SQRT(('1D'!$G$9-'1D'!$G9)^2+('1D'!$H$9-'1D'!$H9)^2)</f>
@@ -2687,61 +2686,61 @@
       </c>
       <c r="I8">
         <f ca="1">SQRT(('1D'!$G$10-'1D'!$G9)^2+('1D'!$H$10-'1D'!$H9)^2)</f>
-        <v>114.39577090203279</v>
+        <v>53.848558516770389</v>
       </c>
       <c r="J8">
         <f ca="1">SQRT(('1D'!$G$11-'1D'!$G9)^2+('1D'!$H$11-'1D'!$H9)^2)</f>
-        <v>37.048149972051064</v>
+        <v>102.45606895448587</v>
       </c>
       <c r="K8">
         <f ca="1">SQRT(('1D'!$G$12-'1D'!$G9)^2+('1D'!$H$12-'1D'!$H9)^2)</f>
-        <v>92.192750141544352</v>
+        <v>53.706075364339533</v>
       </c>
       <c r="L8">
         <f ca="1">SQRT(('1D'!$G$13-'1D'!$G9)^2+('1D'!$H$13-'1D'!$H9)^2)</f>
-        <v>91.597769724438749</v>
+        <v>117.87323087609188</v>
       </c>
       <c r="M8">
         <f ca="1">SQRT(('1D'!$G$14-'1D'!$G9)^2+('1D'!$H$14-'1D'!$H9)^2)</f>
-        <v>49.695791023309205</v>
+        <v>171.97665553964396</v>
       </c>
       <c r="N8">
         <f ca="1">SQRT(('1D'!$G$15-'1D'!$G9)^2+('1D'!$H$15-'1D'!$H9)^2)</f>
-        <v>80.417736119913471</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+        <v>95.806141584750975</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <f ca="1">SQRT(('1D'!$G$2-'1D'!$G10)^2+('1D'!$H$2-'1D'!$H10)^2)</f>
-        <v>63.193720664812389</v>
+        <v>43.880640289053247</v>
       </c>
       <c r="B9">
         <f ca="1">SQRT(('1D'!$G$3-'1D'!$G10)^2+('1D'!$H$3-'1D'!$H10)^2)</f>
-        <v>146.98894228277004</v>
+        <v>103.27573008962048</v>
       </c>
       <c r="C9">
         <f ca="1">SQRT(('1D'!$G$4-'1D'!$G10)^2+('1D'!$H$4-'1D'!$H10)^2)</f>
-        <v>65.346675323777561</v>
+        <v>57.457110591744218</v>
       </c>
       <c r="D9">
         <f ca="1">SQRT(('1D'!$G$5-'1D'!$G10)^2+('1D'!$H$5-'1D'!$H10)^2)</f>
-        <v>86.846256056206684</v>
+        <v>103.49326304060341</v>
       </c>
       <c r="E9">
         <f ca="1">SQRT(('1D'!$G$6-'1D'!$G10)^2+('1D'!$H$6-'1D'!$H10)^2)</f>
-        <v>110.10379424028945</v>
+        <v>108.00343993107724</v>
       </c>
       <c r="F9">
         <f ca="1">SQRT(('1D'!$G$7-'1D'!$G10)^2+('1D'!$H$7-'1D'!$H10)^2)</f>
-        <v>76.2085776283825</v>
+        <v>44.63207006918806</v>
       </c>
       <c r="G9">
         <f ca="1">SQRT(('1D'!$G$8-'1D'!$G10)^2+('1D'!$H$8-'1D'!$H10)^2)</f>
-        <v>77.020518792035219</v>
+        <v>110.13012893779381</v>
       </c>
       <c r="H9">
         <f ca="1">SQRT(('1D'!$G$9-'1D'!$G10)^2+('1D'!$H$9-'1D'!$H10)^2)</f>
-        <v>114.39577090203279</v>
+        <v>53.848558516770389</v>
       </c>
       <c r="I9">
         <f ca="1">SQRT(('1D'!$G$10-'1D'!$G10)^2+('1D'!$H$10-'1D'!$H10)^2)</f>
@@ -2749,61 +2748,61 @@
       </c>
       <c r="J9">
         <f ca="1">SQRT(('1D'!$G$11-'1D'!$G10)^2+('1D'!$H$11-'1D'!$H10)^2)</f>
-        <v>94.095938901913101</v>
+        <v>55.459534018956482</v>
       </c>
       <c r="K9">
         <f ca="1">SQRT(('1D'!$G$12-'1D'!$G10)^2+('1D'!$H$12-'1D'!$H10)^2)</f>
-        <v>38.449696447920203</v>
+        <v>87.327726866909117</v>
       </c>
       <c r="L9">
         <f ca="1">SQRT(('1D'!$G$13-'1D'!$G10)^2+('1D'!$H$13-'1D'!$H10)^2)</f>
-        <v>59.214157501609158</v>
+        <v>68.370109355721894</v>
       </c>
       <c r="M9">
         <f ca="1">SQRT(('1D'!$G$14-'1D'!$G10)^2+('1D'!$H$14-'1D'!$H10)^2)</f>
-        <v>134.97854620540099</v>
+        <v>128.19666341765839</v>
       </c>
       <c r="N9">
         <f ca="1">SQRT(('1D'!$G$15-'1D'!$G10)^2+('1D'!$H$15-'1D'!$H10)^2)</f>
-        <v>63.193720664812389</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <v>43.880640289053247</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <f ca="1">SQRT(('1D'!$G$2-'1D'!$G11)^2+('1D'!$H$2-'1D'!$H11)^2)</f>
-        <v>83.023248745475357</v>
+        <v>19.228690957649487</v>
       </c>
       <c r="B10">
         <f ca="1">SQRT(('1D'!$G$3-'1D'!$G11)^2+('1D'!$H$3-'1D'!$H11)^2)</f>
-        <v>74.749718856626288</v>
+        <v>65.479809736661863</v>
       </c>
       <c r="C10">
         <f ca="1">SQRT(('1D'!$G$4-'1D'!$G11)^2+('1D'!$H$4-'1D'!$H11)^2)</f>
-        <v>129.85302344347599</v>
+        <v>108.04372791773082</v>
       </c>
       <c r="D10">
         <f ca="1">SQRT(('1D'!$G$5-'1D'!$G11)^2+('1D'!$H$5-'1D'!$H11)^2)</f>
-        <v>177.41731488215126</v>
+        <v>51.212064027031523</v>
       </c>
       <c r="E10">
         <f ca="1">SQRT(('1D'!$G$6-'1D'!$G11)^2+('1D'!$H$6-'1D'!$H11)^2)</f>
-        <v>75.635267844973285</v>
+        <v>99.247134468118261</v>
       </c>
       <c r="F10">
         <f ca="1">SQRT(('1D'!$G$7-'1D'!$G11)^2+('1D'!$H$7-'1D'!$H11)^2)</f>
-        <v>149.12933356367384</v>
+        <v>75.313822687553639</v>
       </c>
       <c r="G10">
         <f ca="1">SQRT(('1D'!$G$8-'1D'!$G11)^2+('1D'!$H$8-'1D'!$H11)^2)</f>
-        <v>170.71861230601354</v>
+        <v>54.827462605216674</v>
       </c>
       <c r="H10">
         <f ca="1">SQRT(('1D'!$G$9-'1D'!$G11)^2+('1D'!$H$9-'1D'!$H11)^2)</f>
-        <v>37.048149972051064</v>
+        <v>102.45606895448587</v>
       </c>
       <c r="I10">
         <f ca="1">SQRT(('1D'!$G$10-'1D'!$G11)^2+('1D'!$H$10-'1D'!$H11)^2)</f>
-        <v>94.095938901913101</v>
+        <v>55.459534018956482</v>
       </c>
       <c r="J10">
         <f ca="1">SQRT(('1D'!$G$11-'1D'!$G11)^2+('1D'!$H$11-'1D'!$H11)^2)</f>
@@ -2811,61 +2810,61 @@
       </c>
       <c r="K10">
         <f ca="1">SQRT(('1D'!$G$12-'1D'!$G11)^2+('1D'!$H$12-'1D'!$H11)^2)</f>
-        <v>84.344823035307087</v>
+        <v>142.65110891164008</v>
       </c>
       <c r="L10">
         <f ca="1">SQRT(('1D'!$G$13-'1D'!$G11)^2+('1D'!$H$13-'1D'!$H11)^2)</f>
-        <v>57.400585236320239</v>
+        <v>16.735902462209324</v>
       </c>
       <c r="M10">
         <f ca="1">SQRT(('1D'!$G$14-'1D'!$G11)^2+('1D'!$H$14-'1D'!$H11)^2)</f>
-        <v>84.249869150976906</v>
+        <v>133.24529397528244</v>
       </c>
       <c r="N10">
         <f ca="1">SQRT(('1D'!$G$15-'1D'!$G11)^2+('1D'!$H$15-'1D'!$H11)^2)</f>
-        <v>83.023248745475357</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+        <v>19.228690957649487</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <f ca="1">SQRT(('1D'!$G$2-'1D'!$G12)^2+('1D'!$H$2-'1D'!$H12)^2)</f>
-        <v>24.94105438559567</v>
+        <v>130.48413970297568</v>
       </c>
       <c r="B11">
         <f ca="1">SQRT(('1D'!$G$3-'1D'!$G12)^2+('1D'!$H$3-'1D'!$H12)^2)</f>
-        <v>118.88242556046039</v>
+        <v>184.47303682302626</v>
       </c>
       <c r="C11">
         <f ca="1">SQRT(('1D'!$G$4-'1D'!$G12)^2+('1D'!$H$4-'1D'!$H12)^2)</f>
-        <v>46.260712972264628</v>
+        <v>46.061468591881408</v>
       </c>
       <c r="D11">
         <f ca="1">SQRT(('1D'!$G$5-'1D'!$G12)^2+('1D'!$H$5-'1D'!$H12)^2)</f>
-        <v>97.240386758391494</v>
+        <v>190.32083125474958</v>
       </c>
       <c r="E11">
         <f ca="1">SQRT(('1D'!$G$6-'1D'!$G12)^2+('1D'!$H$6-'1D'!$H12)^2)</f>
-        <v>75.478587366952908</v>
+        <v>159.43552059059502</v>
       </c>
       <c r="F11">
         <f ca="1">SQRT(('1D'!$G$7-'1D'!$G12)^2+('1D'!$H$7-'1D'!$H12)^2)</f>
-        <v>64.861661942952779</v>
+        <v>96.760803748243774</v>
       </c>
       <c r="G11">
         <f ca="1">SQRT(('1D'!$G$8-'1D'!$G12)^2+('1D'!$H$8-'1D'!$H12)^2)</f>
-        <v>103.65873661913729</v>
+        <v>197.42528525581736</v>
       </c>
       <c r="H11">
         <f ca="1">SQRT(('1D'!$G$9-'1D'!$G12)^2+('1D'!$H$9-'1D'!$H12)^2)</f>
-        <v>92.192750141544352</v>
+        <v>53.706075364339533</v>
       </c>
       <c r="I11">
         <f ca="1">SQRT(('1D'!$G$10-'1D'!$G12)^2+('1D'!$H$10-'1D'!$H12)^2)</f>
-        <v>38.449696447920203</v>
+        <v>87.327726866909117</v>
       </c>
       <c r="J11">
         <f ca="1">SQRT(('1D'!$G$11-'1D'!$G12)^2+('1D'!$H$11-'1D'!$H12)^2)</f>
-        <v>84.344823035307087</v>
+        <v>142.65110891164008</v>
       </c>
       <c r="K11">
         <f ca="1">SQRT(('1D'!$G$12-'1D'!$G12)^2+('1D'!$H$12-'1D'!$H12)^2)</f>
@@ -2873,61 +2872,61 @@
       </c>
       <c r="L11">
         <f ca="1">SQRT(('1D'!$G$13-'1D'!$G12)^2+('1D'!$H$13-'1D'!$H12)^2)</f>
-        <v>75.556492123392886</v>
+        <v>155.56401456875631</v>
       </c>
       <c r="M11">
         <f ca="1">SQRT(('1D'!$G$14-'1D'!$G12)^2+('1D'!$H$14-'1D'!$H12)^2)</f>
-        <v>101.60783079637827</v>
+        <v>169.71310433908127</v>
       </c>
       <c r="N11">
         <f ca="1">SQRT(('1D'!$G$15-'1D'!$G12)^2+('1D'!$H$15-'1D'!$H12)^2)</f>
-        <v>24.94105438559567</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+        <v>130.48413970297568</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <f ca="1">SQRT(('1D'!$G$2-'1D'!$G13)^2+('1D'!$H$2-'1D'!$H13)^2)</f>
-        <v>90.656939655835203</v>
+        <v>25.648770097635538</v>
       </c>
       <c r="B12">
         <f ca="1">SQRT(('1D'!$G$3-'1D'!$G13)^2+('1D'!$H$3-'1D'!$H13)^2)</f>
-        <v>129.65074433219556</v>
+        <v>49.85791641435204</v>
       </c>
       <c r="C12">
         <f ca="1">SQRT(('1D'!$G$4-'1D'!$G13)^2+('1D'!$H$4-'1D'!$H13)^2)</f>
-        <v>118.22655745351892</v>
+        <v>123.12746260042005</v>
       </c>
       <c r="D12">
         <f ca="1">SQRT(('1D'!$G$5-'1D'!$G13)^2+('1D'!$H$5-'1D'!$H13)^2)</f>
-        <v>145.17117761756396</v>
+        <v>35.505798315262069</v>
       </c>
       <c r="E12">
         <f ca="1">SQRT(('1D'!$G$6-'1D'!$G13)^2+('1D'!$H$6-'1D'!$H13)^2)</f>
-        <v>113.79831003666696</v>
+        <v>112.79721813747902</v>
       </c>
       <c r="F12">
         <f ca="1">SQRT(('1D'!$G$7-'1D'!$G13)^2+('1D'!$H$7-'1D'!$H13)^2)</f>
-        <v>132.85159532401258</v>
+        <v>79.729514652613119</v>
       </c>
       <c r="G12">
         <f ca="1">SQRT(('1D'!$G$8-'1D'!$G13)^2+('1D'!$H$8-'1D'!$H13)^2)</f>
-        <v>126.74521795027334</v>
+        <v>43.039673049034562</v>
       </c>
       <c r="H12">
         <f ca="1">SQRT(('1D'!$G$9-'1D'!$G13)^2+('1D'!$H$9-'1D'!$H13)^2)</f>
-        <v>91.597769724438749</v>
+        <v>117.87323087609188</v>
       </c>
       <c r="I12">
         <f ca="1">SQRT(('1D'!$G$10-'1D'!$G13)^2+('1D'!$H$10-'1D'!$H13)^2)</f>
-        <v>59.214157501609158</v>
+        <v>68.370109355721894</v>
       </c>
       <c r="J12">
         <f ca="1">SQRT(('1D'!$G$11-'1D'!$G13)^2+('1D'!$H$11-'1D'!$H13)^2)</f>
-        <v>57.400585236320239</v>
+        <v>16.735902462209324</v>
       </c>
       <c r="K12">
         <f ca="1">SQRT(('1D'!$G$12-'1D'!$G13)^2+('1D'!$H$12-'1D'!$H13)^2)</f>
-        <v>75.556492123392886</v>
+        <v>155.56401456875631</v>
       </c>
       <c r="L12">
         <f ca="1">SQRT(('1D'!$G$13-'1D'!$G13)^2+('1D'!$H$13-'1D'!$H13)^2)</f>
@@ -2935,61 +2934,61 @@
       </c>
       <c r="M12">
         <f ca="1">SQRT(('1D'!$G$14-'1D'!$G13)^2+('1D'!$H$14-'1D'!$H13)^2)</f>
-        <v>131.30912263393097</v>
+        <v>126.41008335974669</v>
       </c>
       <c r="N12">
         <f ca="1">SQRT(('1D'!$G$15-'1D'!$G13)^2+('1D'!$H$15-'1D'!$H13)^2)</f>
-        <v>90.656939655835203</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+        <v>25.648770097635538</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <f ca="1">SQRT(('1D'!$G$2-'1D'!$G14)^2+('1D'!$H$2-'1D'!$H14)^2)</f>
-        <v>79.832065176193368</v>
+        <v>116.64427352380943</v>
       </c>
       <c r="B13">
         <f ca="1">SQRT(('1D'!$G$3-'1D'!$G14)^2+('1D'!$H$3-'1D'!$H14)^2)</f>
-        <v>32.252090312264833</v>
+        <v>97.793687081700568</v>
       </c>
       <c r="C13">
         <f ca="1">SQRT(('1D'!$G$4-'1D'!$G14)^2+('1D'!$H$4-'1D'!$H14)^2)</f>
-        <v>127.7624184174953</v>
+        <v>171.40127831996497</v>
       </c>
       <c r="D13">
         <f ca="1">SQRT(('1D'!$G$5-'1D'!$G14)^2+('1D'!$H$5-'1D'!$H14)^2)</f>
-        <v>192.84623526199829</v>
+        <v>133.52260781850461</v>
       </c>
       <c r="E13">
         <f ca="1">SQRT(('1D'!$G$6-'1D'!$G14)^2+('1D'!$H$6-'1D'!$H14)^2)</f>
-        <v>26.601281287280955</v>
+        <v>227.57101082443432</v>
       </c>
       <c r="F13">
         <f ca="1">SQRT(('1D'!$G$7-'1D'!$G14)^2+('1D'!$H$7-'1D'!$H14)^2)</f>
-        <v>147.59606209539737</v>
+        <v>85.604184160602358</v>
       </c>
       <c r="G13">
         <f ca="1">SQRT(('1D'!$G$8-'1D'!$G14)^2+('1D'!$H$8-'1D'!$H14)^2)</f>
-        <v>205.1918724307157</v>
+        <v>153.60926816178537</v>
       </c>
       <c r="H13">
         <f ca="1">SQRT(('1D'!$G$9-'1D'!$G14)^2+('1D'!$H$9-'1D'!$H14)^2)</f>
-        <v>49.695791023309205</v>
+        <v>171.97665553964396</v>
       </c>
       <c r="I13">
         <f ca="1">SQRT(('1D'!$G$10-'1D'!$G14)^2+('1D'!$H$10-'1D'!$H14)^2)</f>
-        <v>134.97854620540099</v>
+        <v>128.19666341765839</v>
       </c>
       <c r="J13">
         <f ca="1">SQRT(('1D'!$G$11-'1D'!$G14)^2+('1D'!$H$11-'1D'!$H14)^2)</f>
-        <v>84.249869150976906</v>
+        <v>133.24529397528244</v>
       </c>
       <c r="K13">
         <f ca="1">SQRT(('1D'!$G$12-'1D'!$G14)^2+('1D'!$H$12-'1D'!$H14)^2)</f>
-        <v>101.60783079637827</v>
+        <v>169.71310433908127</v>
       </c>
       <c r="L13">
         <f ca="1">SQRT(('1D'!$G$13-'1D'!$G14)^2+('1D'!$H$13-'1D'!$H14)^2)</f>
-        <v>131.30912263393097</v>
+        <v>126.41008335974669</v>
       </c>
       <c r="M13">
         <f ca="1">SQRT(('1D'!$G$14-'1D'!$G14)^2+('1D'!$H$14-'1D'!$H14)^2)</f>
@@ -2997,61 +2996,61 @@
       </c>
       <c r="N13">
         <f ca="1">SQRT(('1D'!$G$15-'1D'!$G14)^2+('1D'!$H$15-'1D'!$H14)^2)</f>
-        <v>79.832065176193368</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+        <v>116.64427352380943</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>SQRT(('1D'!$G$2-'1D'!$G15)^2+('1D'!$H$2-'1D'!$H15)^2)</f>
         <v>0</v>
       </c>
       <c r="B14">
         <f ca="1">SQRT(('1D'!$G$3-'1D'!$G15)^2+('1D'!$H$3-'1D'!$H15)^2)</f>
-        <v>100.98318659323294</v>
+        <v>62.450294483102191</v>
       </c>
       <c r="C14">
         <f ca="1">SQRT(('1D'!$G$4-'1D'!$G15)^2+('1D'!$H$4-'1D'!$H15)^2)</f>
-        <v>52.052742328235517</v>
+        <v>100.38253739063121</v>
       </c>
       <c r="D14">
         <f ca="1">SQRT(('1D'!$G$5-'1D'!$G15)^2+('1D'!$H$5-'1D'!$H15)^2)</f>
-        <v>113.77242934243556</v>
+        <v>59.840809797133609</v>
       </c>
       <c r="E14">
         <f ca="1">SQRT(('1D'!$G$6-'1D'!$G15)^2+('1D'!$H$6-'1D'!$H15)^2)</f>
-        <v>53.24550785526278</v>
+        <v>112.10717392214546</v>
       </c>
       <c r="F14">
         <f ca="1">SQRT(('1D'!$G$7-'1D'!$G15)^2+('1D'!$H$7-'1D'!$H15)^2)</f>
-        <v>72.599533148136715</v>
+        <v>56.36935416048393</v>
       </c>
       <c r="G14">
         <f ca="1">SQRT(('1D'!$G$8-'1D'!$G15)^2+('1D'!$H$8-'1D'!$H15)^2)</f>
-        <v>126.11704105830356</v>
+        <v>68.647024002803633</v>
       </c>
       <c r="H14">
         <f ca="1">SQRT(('1D'!$G$9-'1D'!$G15)^2+('1D'!$H$9-'1D'!$H15)^2)</f>
-        <v>80.417736119913471</v>
+        <v>95.806141584750975</v>
       </c>
       <c r="I14">
         <f ca="1">SQRT(('1D'!$G$10-'1D'!$G15)^2+('1D'!$H$10-'1D'!$H15)^2)</f>
-        <v>63.193720664812389</v>
+        <v>43.880640289053247</v>
       </c>
       <c r="J14">
         <f ca="1">SQRT(('1D'!$G$11-'1D'!$G15)^2+('1D'!$H$11-'1D'!$H15)^2)</f>
-        <v>83.023248745475357</v>
+        <v>19.228690957649487</v>
       </c>
       <c r="K14">
         <f ca="1">SQRT(('1D'!$G$12-'1D'!$G15)^2+('1D'!$H$12-'1D'!$H15)^2)</f>
-        <v>24.94105438559567</v>
+        <v>130.48413970297568</v>
       </c>
       <c r="L14">
         <f ca="1">SQRT(('1D'!$G$13-'1D'!$G15)^2+('1D'!$H$13-'1D'!$H15)^2)</f>
-        <v>90.656939655835203</v>
+        <v>25.648770097635538</v>
       </c>
       <c r="M14">
         <f ca="1">SQRT(('1D'!$G$14-'1D'!$G15)^2+('1D'!$H$14-'1D'!$H15)^2)</f>
-        <v>79.832065176193368</v>
+        <v>116.64427352380943</v>
       </c>
       <c r="N14">
         <f>SQRT(('1D'!$G$15-'1D'!$G15)^2+('1D'!$H$15-'1D'!$H15)^2)</f>
@@ -3070,64 +3069,64 @@
   </sheetPr>
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>Distances!A1/80</f>
         <v>0</v>
       </c>
       <c r="B1">
         <f ca="1">Distances!B1/80</f>
-        <v>1.2622898324154117</v>
+        <v>0.78062868103877736</v>
       </c>
       <c r="C1">
         <f ca="1">Distances!C1/80</f>
-        <v>0.65065927910294397</v>
+        <v>1.2547817173828901</v>
       </c>
       <c r="D1">
         <f ca="1">Distances!D1/80</f>
-        <v>1.4221553667804445</v>
+        <v>0.74801012246417009</v>
       </c>
       <c r="E1">
+        <f ca="1">Distances!E1/80</f>
+        <v>1.4013396740268182</v>
+      </c>
+      <c r="F1">
         <f ca="1">Distances!F1/80</f>
-        <v>0.90749416435170893</v>
-      </c>
-      <c r="F1">
-        <f ca="1">Distances!G1/80</f>
-        <v>1.5764630132287945</v>
+        <v>0.70461692700604917</v>
       </c>
       <c r="G1">
         <f ca="1">Distances!G1/80</f>
-        <v>1.5764630132287945</v>
+        <v>0.85808780003504537</v>
       </c>
       <c r="H1">
         <f ca="1">Distances!H1/80</f>
-        <v>1.0052217014989184</v>
+        <v>1.1975767698093871</v>
       </c>
       <c r="I1">
         <f ca="1">Distances!I1/80</f>
-        <v>0.78992150831015484</v>
+        <v>0.54850800361316554</v>
       </c>
       <c r="J1">
         <f ca="1">Distances!J1/80</f>
-        <v>1.0377906093184419</v>
+        <v>0.2403586369706186</v>
       </c>
       <c r="K1">
         <f ca="1">Distances!K1/80</f>
-        <v>0.31176317981994589</v>
+        <v>1.6310517462871961</v>
       </c>
       <c r="L1">
         <f ca="1">Distances!L1/80</f>
-        <v>1.13321174569794</v>
+        <v>0.3206096262204442</v>
       </c>
       <c r="M1">
         <f ca="1">Distances!M1/80</f>
-        <v>0.99790081470241709</v>
+        <v>1.458053419047618</v>
       </c>
       <c r="N1">
         <f>Distances!N1/80</f>
@@ -3146,10 +3145,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <f ca="1">Distances!A2/80</f>
-        <v>1.2622898324154117</v>
+        <v>0.78062868103877736</v>
       </c>
       <c r="B2">
         <f ca="1">Distances!B2/80</f>
@@ -3157,51 +3156,51 @@
       </c>
       <c r="C2">
         <f ca="1">Distances!C2/80</f>
-        <v>1.9004879119309177</v>
+        <v>2.0091362163426587</v>
       </c>
       <c r="D2">
         <f ca="1">Distances!D2/80</f>
-        <v>2.681606168886093</v>
+        <v>0.46920150222618562</v>
       </c>
       <c r="E2">
         <f ca="1">Distances!E2/80</f>
-        <v>0.65125522151331205</v>
+        <v>2.0277135928164713</v>
       </c>
       <c r="F2">
         <f ca="1">Distances!F2/80</f>
-        <v>2.1553876047236011</v>
+        <v>1.1470004546053854</v>
       </c>
       <c r="G2">
         <f ca="1">Distances!G2/80</f>
-        <v>2.7686838004561491</v>
+        <v>0.72525694988304501</v>
       </c>
       <c r="H2">
         <f ca="1">Distances!H2/80</f>
-        <v>0.47695788103933712</v>
+        <v>1.9612832606791071</v>
       </c>
       <c r="I2">
         <f ca="1">Distances!I2/80</f>
-        <v>1.8373617785346255</v>
+        <v>1.290946626120256</v>
       </c>
       <c r="J2">
         <f ca="1">Distances!J2/80</f>
-        <v>0.93437148570782858</v>
+        <v>0.81849762170827334</v>
       </c>
       <c r="K2">
         <f ca="1">Distances!K2/80</f>
-        <v>1.4860303195057549</v>
+        <v>2.3059129602878281</v>
       </c>
       <c r="L2">
         <f ca="1">Distances!L2/80</f>
-        <v>1.6206343041524445</v>
+        <v>0.62322395517940055</v>
       </c>
       <c r="M2">
         <f ca="1">Distances!M2/80</f>
-        <v>0.4031511289033104</v>
+        <v>1.2224210885212572</v>
       </c>
       <c r="N2">
         <f ca="1">Distances!N2/80</f>
-        <v>1.2622898324154117</v>
+        <v>0.78062868103877736</v>
       </c>
       <c r="O2">
         <f>Distances!O2/80</f>
@@ -3216,14 +3215,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <f ca="1">Distances!A3/80</f>
-        <v>0.65065927910294397</v>
+        <v>1.2547817173828901</v>
       </c>
       <c r="B3">
         <f ca="1">Distances!B3/80</f>
-        <v>1.9004879119309177</v>
+        <v>2.0091362163426587</v>
       </c>
       <c r="C3">
         <f ca="1">Distances!C3/80</f>
@@ -3231,47 +3230,47 @@
       </c>
       <c r="D3">
         <f ca="1">Distances!D3/80</f>
-        <v>0.83488769720955447</v>
+        <v>1.9829019735708429</v>
       </c>
       <c r="E3">
         <f ca="1">Distances!E3/80</f>
-        <v>1.2708535666531273</v>
+        <v>1.4183574616457437</v>
       </c>
       <c r="F3">
         <f ca="1">Distances!F3/80</f>
-        <v>0.25689857278840789</v>
+        <v>1.0900313048419403</v>
       </c>
       <c r="G3">
         <f ca="1">Distances!G3/80</f>
-        <v>1.1512445195532353</v>
+        <v>2.0273796776556128</v>
       </c>
       <c r="H3">
         <f ca="1">Distances!H3/80</f>
-        <v>1.6531574433075746</v>
+        <v>9.6142028082953968E-2</v>
       </c>
       <c r="I3">
         <f ca="1">Distances!I3/80</f>
-        <v>0.81683344154721949</v>
+        <v>0.71821388239680273</v>
       </c>
       <c r="J3">
         <f ca="1">Distances!J3/80</f>
-        <v>1.6231627930434498</v>
+        <v>1.3505465989716352</v>
       </c>
       <c r="K3">
         <f ca="1">Distances!K3/80</f>
-        <v>0.57825891215330782</v>
+        <v>0.57576835739851762</v>
       </c>
       <c r="L3">
         <f ca="1">Distances!L3/80</f>
-        <v>1.4778319681689864</v>
+        <v>1.5390932825052506</v>
       </c>
       <c r="M3">
         <f ca="1">Distances!M3/80</f>
-        <v>1.5970302302186912</v>
+        <v>2.1425159789995623</v>
       </c>
       <c r="N3">
         <f ca="1">Distances!N3/80</f>
-        <v>0.65065927910294397</v>
+        <v>1.2547817173828901</v>
       </c>
       <c r="O3">
         <f>Distances!O3/80</f>
@@ -3286,18 +3285,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <f ca="1">Distances!A4/80</f>
-        <v>1.4221553667804445</v>
+        <v>0.74801012246417009</v>
       </c>
       <c r="B4">
         <f ca="1">Distances!B4/80</f>
-        <v>2.681606168886093</v>
+        <v>0.46920150222618562</v>
       </c>
       <c r="C4">
         <f ca="1">Distances!C4/80</f>
-        <v>0.83488769720955447</v>
+        <v>1.9829019735708429</v>
       </c>
       <c r="D4">
         <f ca="1">Distances!D4/80</f>
@@ -3305,43 +3304,43 @@
       </c>
       <c r="E4">
         <f ca="1">Distances!E4/80</f>
-        <v>2.0792514086994887</v>
+        <v>1.6887186224452679</v>
       </c>
       <c r="F4">
         <f ca="1">Distances!F4/80</f>
-        <v>0.63299703455039114</v>
+        <v>1.3500605149774656</v>
       </c>
       <c r="G4">
         <f ca="1">Distances!G4/80</f>
-        <v>0.55214012625838982</v>
+        <v>0.25625487425325372</v>
       </c>
       <c r="H4">
         <f ca="1">Distances!H4/80</f>
-        <v>2.3678297471736163</v>
+        <v>1.9167111820514893</v>
       </c>
       <c r="I4">
         <f ca="1">Distances!I4/80</f>
-        <v>1.0855782007025836</v>
+        <v>1.2936657880075426</v>
       </c>
       <c r="J4">
         <f ca="1">Distances!J4/80</f>
-        <v>2.2177164360268908</v>
+        <v>0.64015080033789407</v>
       </c>
       <c r="K4">
         <f ca="1">Distances!K4/80</f>
-        <v>1.2155048344798938</v>
+        <v>2.3790103906843698</v>
       </c>
       <c r="L4">
         <f ca="1">Distances!L4/80</f>
-        <v>1.8146397202195494</v>
+        <v>0.44382247894077587</v>
       </c>
       <c r="M4">
         <f ca="1">Distances!M4/80</f>
-        <v>2.4105779407749788</v>
+        <v>1.6690325977313076</v>
       </c>
       <c r="N4">
         <f ca="1">Distances!N4/80</f>
-        <v>1.4221553667804445</v>
+        <v>0.74801012246417009</v>
       </c>
       <c r="O4">
         <f>Distances!O4/80</f>
@@ -3356,22 +3355,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <f ca="1">Distances!A5/80</f>
-        <v>0.66556884819078477</v>
+        <v>1.4013396740268182</v>
       </c>
       <c r="B5">
         <f ca="1">Distances!B5/80</f>
-        <v>0.65125522151331205</v>
+        <v>2.0277135928164713</v>
       </c>
       <c r="C5">
         <f ca="1">Distances!C5/80</f>
-        <v>1.2708535666531273</v>
+        <v>1.4183574616457437</v>
       </c>
       <c r="D5">
         <f ca="1">Distances!D5/80</f>
-        <v>2.0792514086994887</v>
+        <v>1.6887186224452679</v>
       </c>
       <c r="E5">
         <f ca="1">Distances!E5/80</f>
@@ -3379,39 +3378,39 @@
       </c>
       <c r="F5">
         <f ca="1">Distances!F5/80</f>
-        <v>1.5216091426504197</v>
+        <v>1.8904496825728074</v>
       </c>
       <c r="G5">
         <f ca="1">Distances!G5/80</f>
-        <v>2.2358579773336764</v>
+        <v>1.5434754324054085</v>
       </c>
       <c r="H5">
         <f ca="1">Distances!H5/80</f>
-        <v>0.61928233667889332</v>
+        <v>1.324171319244845</v>
       </c>
       <c r="I5">
         <f ca="1">Distances!I5/80</f>
-        <v>1.376297428003618</v>
+        <v>1.3500429991384655</v>
       </c>
       <c r="J5">
         <f ca="1">Distances!J5/80</f>
-        <v>0.94544084806216611</v>
+        <v>1.2405891808514782</v>
       </c>
       <c r="K5">
         <f ca="1">Distances!K5/80</f>
-        <v>0.9434823420869114</v>
+        <v>1.9929440073824378</v>
       </c>
       <c r="L5">
         <f ca="1">Distances!L5/80</f>
-        <v>1.4224788754583371</v>
+        <v>1.4099652267184877</v>
       </c>
       <c r="M5">
         <f ca="1">Distances!M5/80</f>
-        <v>0.33251601609101195</v>
+        <v>2.8446376353054292</v>
       </c>
       <c r="N5">
         <f ca="1">Distances!N5/80</f>
-        <v>0.66556884819078477</v>
+        <v>1.4013396740268182</v>
       </c>
       <c r="O5">
         <f>Distances!O5/80</f>
@@ -3426,26 +3425,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <f ca="1">Distances!A6/80</f>
-        <v>0.90749416435170893</v>
+        <v>0.70461692700604917</v>
       </c>
       <c r="B6">
         <f ca="1">Distances!B6/80</f>
-        <v>2.1553876047236011</v>
+        <v>1.1470004546053854</v>
       </c>
       <c r="C6">
         <f ca="1">Distances!C6/80</f>
-        <v>0.25689857278840789</v>
+        <v>1.0900313048419403</v>
       </c>
       <c r="D6">
         <f ca="1">Distances!D6/80</f>
-        <v>0.63299703455039114</v>
+        <v>1.3500605149774656</v>
       </c>
       <c r="E6">
         <f ca="1">Distances!E6/80</f>
-        <v>1.5216091426504197</v>
+        <v>1.8904496825728074</v>
       </c>
       <c r="F6">
         <f ca="1">Distances!F6/80</f>
@@ -3453,35 +3452,35 @@
       </c>
       <c r="G6">
         <f ca="1">Distances!G6/80</f>
-        <v>1.042650703432332</v>
+        <v>1.5207890022873536</v>
       </c>
       <c r="H6">
         <f ca="1">Distances!H6/80</f>
-        <v>1.9089972839579652</v>
+        <v>1.0871670198994186</v>
       </c>
       <c r="I6">
         <f ca="1">Distances!I6/80</f>
-        <v>0.95260722035478129</v>
+        <v>0.55790087586485071</v>
       </c>
       <c r="J6">
         <f ca="1">Distances!J6/80</f>
-        <v>1.864116669545923</v>
+        <v>0.94142278359442044</v>
       </c>
       <c r="K6">
         <f ca="1">Distances!K6/80</f>
-        <v>0.81077077428690969</v>
+        <v>1.2095100468530471</v>
       </c>
       <c r="L6">
         <f ca="1">Distances!L6/80</f>
-        <v>1.6606449415501572</v>
+        <v>0.99661893315766403</v>
       </c>
       <c r="M6">
         <f ca="1">Distances!M6/80</f>
-        <v>1.8449507761924671</v>
+        <v>1.0700523020075294</v>
       </c>
       <c r="N6">
         <f ca="1">Distances!N6/80</f>
-        <v>0.90749416435170893</v>
+        <v>0.70461692700604917</v>
       </c>
       <c r="O6">
         <f>Distances!O6/80</f>
@@ -3496,30 +3495,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <f ca="1">Distances!A7/80</f>
-        <v>1.5764630132287945</v>
+        <v>0.85808780003504537</v>
       </c>
       <c r="B7">
         <f ca="1">Distances!B7/80</f>
-        <v>2.7686838004561491</v>
+        <v>0.72525694988304501</v>
       </c>
       <c r="C7">
         <f ca="1">Distances!C7/80</f>
-        <v>1.1512445195532353</v>
+        <v>2.0273796776556128</v>
       </c>
       <c r="D7">
         <f ca="1">Distances!D7/80</f>
-        <v>0.55214012625838982</v>
+        <v>0.25625487425325372</v>
       </c>
       <c r="E7">
         <f ca="1">Distances!E7/80</f>
-        <v>2.2358579773336764</v>
+        <v>1.5434754324054085</v>
       </c>
       <c r="F7">
         <f ca="1">Distances!F7/80</f>
-        <v>1.042650703432332</v>
+        <v>1.5207890022873536</v>
       </c>
       <c r="G7">
         <f ca="1">Distances!G7/80</f>
@@ -3527,31 +3526,31 @@
       </c>
       <c r="H7">
         <f ca="1">Distances!H7/80</f>
-        <v>2.3850890283578985</v>
+        <v>1.9527942548557076</v>
       </c>
       <c r="I7">
         <f ca="1">Distances!I7/80</f>
-        <v>0.96275648490044019</v>
+        <v>1.3766266117224226</v>
       </c>
       <c r="J7">
         <f ca="1">Distances!J7/80</f>
-        <v>2.1339826538251692</v>
+        <v>0.68534328256520838</v>
       </c>
       <c r="K7">
         <f ca="1">Distances!K7/80</f>
-        <v>1.295734207739216</v>
+        <v>2.4678160656977171</v>
       </c>
       <c r="L7">
         <f ca="1">Distances!L7/80</f>
-        <v>1.5843152243784169</v>
+        <v>0.53799591311293204</v>
       </c>
       <c r="M7">
         <f ca="1">Distances!M7/80</f>
-        <v>2.5648984053839463</v>
+        <v>1.9201158520223172</v>
       </c>
       <c r="N7">
         <f ca="1">Distances!N7/80</f>
-        <v>1.5764630132287945</v>
+        <v>0.85808780003504537</v>
       </c>
       <c r="O7">
         <f>Distances!O7/80</f>
@@ -3566,34 +3565,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <f ca="1">Distances!A8/80</f>
-        <v>1.0052217014989184</v>
+        <v>1.1975767698093871</v>
       </c>
       <c r="B8">
         <f ca="1">Distances!B8/80</f>
-        <v>0.47695788103933712</v>
+        <v>1.9612832606791071</v>
       </c>
       <c r="C8">
         <f ca="1">Distances!C8/80</f>
-        <v>1.6531574433075746</v>
+        <v>9.6142028082953968E-2</v>
       </c>
       <c r="D8">
         <f ca="1">Distances!D8/80</f>
-        <v>2.3678297471736163</v>
+        <v>1.9167111820514893</v>
       </c>
       <c r="E8">
         <f ca="1">Distances!E8/80</f>
-        <v>0.61928233667889332</v>
+        <v>1.324171319244845</v>
       </c>
       <c r="F8">
         <f ca="1">Distances!F8/80</f>
-        <v>1.9089972839579652</v>
+        <v>1.0871670198994186</v>
       </c>
       <c r="G8">
         <f ca="1">Distances!G8/80</f>
-        <v>2.3850890283578985</v>
+        <v>1.9527942548557076</v>
       </c>
       <c r="H8">
         <f ca="1">Distances!H8/80</f>
@@ -3601,27 +3600,27 @@
       </c>
       <c r="I8">
         <f ca="1">Distances!I8/80</f>
-        <v>1.4299471362754099</v>
+        <v>0.67310698145962988</v>
       </c>
       <c r="J8">
         <f ca="1">Distances!J8/80</f>
-        <v>0.46310187465063829</v>
+        <v>1.2807008619310734</v>
       </c>
       <c r="K8">
         <f ca="1">Distances!K8/80</f>
-        <v>1.1524093767693044</v>
+        <v>0.67132594205424412</v>
       </c>
       <c r="L8">
         <f ca="1">Distances!L8/80</f>
-        <v>1.1449721215554844</v>
+        <v>1.4734153859511485</v>
       </c>
       <c r="M8">
         <f ca="1">Distances!M8/80</f>
-        <v>0.62119738779136502</v>
+        <v>2.1497081942455494</v>
       </c>
       <c r="N8">
         <f ca="1">Distances!N8/80</f>
-        <v>1.0052217014989184</v>
+        <v>1.1975767698093871</v>
       </c>
       <c r="O8">
         <f>Distances!O8/80</f>
@@ -3636,38 +3635,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <f ca="1">Distances!A9/80</f>
-        <v>0.78992150831015484</v>
+        <v>0.54850800361316554</v>
       </c>
       <c r="B9">
         <f ca="1">Distances!B9/80</f>
-        <v>1.8373617785346255</v>
+        <v>1.290946626120256</v>
       </c>
       <c r="C9">
         <f ca="1">Distances!C9/80</f>
-        <v>0.81683344154721949</v>
+        <v>0.71821388239680273</v>
       </c>
       <c r="D9">
         <f ca="1">Distances!D9/80</f>
-        <v>1.0855782007025836</v>
+        <v>1.2936657880075426</v>
       </c>
       <c r="E9">
         <f ca="1">Distances!E9/80</f>
-        <v>1.376297428003618</v>
+        <v>1.3500429991384655</v>
       </c>
       <c r="F9">
         <f ca="1">Distances!F9/80</f>
-        <v>0.95260722035478129</v>
+        <v>0.55790087586485071</v>
       </c>
       <c r="G9">
         <f ca="1">Distances!G9/80</f>
-        <v>0.96275648490044019</v>
+        <v>1.3766266117224226</v>
       </c>
       <c r="H9">
         <f ca="1">Distances!H9/80</f>
-        <v>1.4299471362754099</v>
+        <v>0.67310698145962988</v>
       </c>
       <c r="I9">
         <f ca="1">Distances!I9/80</f>
@@ -3675,23 +3674,23 @@
       </c>
       <c r="J9">
         <f ca="1">Distances!J9/80</f>
-        <v>1.1761992362739138</v>
+        <v>0.69324417523695603</v>
       </c>
       <c r="K9">
         <f ca="1">Distances!K9/80</f>
-        <v>0.48062120559900257</v>
+        <v>1.0915965858363639</v>
       </c>
       <c r="L9">
         <f ca="1">Distances!L9/80</f>
-        <v>0.74017696877011452</v>
+        <v>0.85462636694652372</v>
       </c>
       <c r="M9">
         <f ca="1">Distances!M9/80</f>
-        <v>1.6872318275675124</v>
+        <v>1.6024582927207298</v>
       </c>
       <c r="N9">
         <f ca="1">Distances!N9/80</f>
-        <v>0.78992150831015484</v>
+        <v>0.54850800361316554</v>
       </c>
       <c r="O9">
         <f>Distances!O9/80</f>
@@ -3706,42 +3705,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <f ca="1">Distances!A10/80</f>
-        <v>1.0377906093184419</v>
+        <v>0.2403586369706186</v>
       </c>
       <c r="B10">
         <f ca="1">Distances!B10/80</f>
-        <v>0.93437148570782858</v>
+        <v>0.81849762170827334</v>
       </c>
       <c r="C10">
         <f ca="1">Distances!C10/80</f>
-        <v>1.6231627930434498</v>
+        <v>1.3505465989716352</v>
       </c>
       <c r="D10">
         <f ca="1">Distances!D10/80</f>
-        <v>2.2177164360268908</v>
+        <v>0.64015080033789407</v>
       </c>
       <c r="E10">
         <f ca="1">Distances!E10/80</f>
-        <v>0.94544084806216611</v>
+        <v>1.2405891808514782</v>
       </c>
       <c r="F10">
         <f ca="1">Distances!F10/80</f>
-        <v>1.864116669545923</v>
+        <v>0.94142278359442044</v>
       </c>
       <c r="G10">
         <f ca="1">Distances!G10/80</f>
-        <v>2.1339826538251692</v>
+        <v>0.68534328256520838</v>
       </c>
       <c r="H10">
         <f ca="1">Distances!H10/80</f>
-        <v>0.46310187465063829</v>
+        <v>1.2807008619310734</v>
       </c>
       <c r="I10">
         <f ca="1">Distances!I10/80</f>
-        <v>1.1761992362739138</v>
+        <v>0.69324417523695603</v>
       </c>
       <c r="J10">
         <f ca="1">Distances!J10/80</f>
@@ -3749,19 +3748,19 @@
       </c>
       <c r="K10">
         <f ca="1">Distances!K10/80</f>
-        <v>1.0543102879413386</v>
+        <v>1.783138861395501</v>
       </c>
       <c r="L10">
         <f ca="1">Distances!L10/80</f>
-        <v>0.71750731545400304</v>
+        <v>0.20919878077761656</v>
       </c>
       <c r="M10">
         <f ca="1">Distances!M10/80</f>
-        <v>1.0531233643872113</v>
+        <v>1.6655661746910304</v>
       </c>
       <c r="N10">
         <f ca="1">Distances!N10/80</f>
-        <v>1.0377906093184419</v>
+        <v>0.2403586369706186</v>
       </c>
       <c r="O10">
         <f>Distances!O10/80</f>
@@ -3776,46 +3775,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <f ca="1">Distances!A11/80</f>
-        <v>0.31176317981994589</v>
+        <v>1.6310517462871961</v>
       </c>
       <c r="B11">
         <f ca="1">Distances!B11/80</f>
-        <v>1.4860303195057549</v>
+        <v>2.3059129602878281</v>
       </c>
       <c r="C11">
         <f ca="1">Distances!C11/80</f>
-        <v>0.57825891215330782</v>
+        <v>0.57576835739851762</v>
       </c>
       <c r="D11">
         <f ca="1">Distances!D11/80</f>
-        <v>1.2155048344798938</v>
+        <v>2.3790103906843698</v>
       </c>
       <c r="E11">
         <f ca="1">Distances!E11/80</f>
-        <v>0.9434823420869114</v>
+        <v>1.9929440073824378</v>
       </c>
       <c r="F11">
         <f ca="1">Distances!F11/80</f>
-        <v>0.81077077428690969</v>
+        <v>1.2095100468530471</v>
       </c>
       <c r="G11">
         <f ca="1">Distances!G11/80</f>
-        <v>1.295734207739216</v>
+        <v>2.4678160656977171</v>
       </c>
       <c r="H11">
         <f ca="1">Distances!H11/80</f>
-        <v>1.1524093767693044</v>
+        <v>0.67132594205424412</v>
       </c>
       <c r="I11">
         <f ca="1">Distances!I11/80</f>
-        <v>0.48062120559900257</v>
+        <v>1.0915965858363639</v>
       </c>
       <c r="J11">
         <f ca="1">Distances!J11/80</f>
-        <v>1.0543102879413386</v>
+        <v>1.783138861395501</v>
       </c>
       <c r="K11">
         <f ca="1">Distances!K11/80</f>
@@ -3823,15 +3822,15 @@
       </c>
       <c r="L11">
         <f ca="1">Distances!L11/80</f>
-        <v>0.94445615154241103</v>
+        <v>1.9445501821094537</v>
       </c>
       <c r="M11">
         <f ca="1">Distances!M11/80</f>
-        <v>1.2700978849547284</v>
+        <v>2.1214138042385158</v>
       </c>
       <c r="N11">
         <f ca="1">Distances!N11/80</f>
-        <v>0.31176317981994589</v>
+        <v>1.6310517462871961</v>
       </c>
       <c r="O11">
         <f>Distances!O11/80</f>
@@ -3846,50 +3845,50 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <f ca="1">Distances!A12/80</f>
-        <v>1.13321174569794</v>
+        <v>0.3206096262204442</v>
       </c>
       <c r="B12">
         <f ca="1">Distances!B12/80</f>
-        <v>1.6206343041524445</v>
+        <v>0.62322395517940055</v>
       </c>
       <c r="C12">
         <f ca="1">Distances!C12/80</f>
-        <v>1.4778319681689864</v>
+        <v>1.5390932825052506</v>
       </c>
       <c r="D12">
         <f ca="1">Distances!D12/80</f>
-        <v>1.8146397202195494</v>
+        <v>0.44382247894077587</v>
       </c>
       <c r="E12">
         <f ca="1">Distances!E12/80</f>
-        <v>1.4224788754583371</v>
+        <v>1.4099652267184877</v>
       </c>
       <c r="F12">
         <f ca="1">Distances!F12/80</f>
-        <v>1.6606449415501572</v>
+        <v>0.99661893315766403</v>
       </c>
       <c r="G12">
         <f ca="1">Distances!G12/80</f>
-        <v>1.5843152243784169</v>
+        <v>0.53799591311293204</v>
       </c>
       <c r="H12">
         <f ca="1">Distances!H12/80</f>
-        <v>1.1449721215554844</v>
+        <v>1.4734153859511485</v>
       </c>
       <c r="I12">
         <f ca="1">Distances!I12/80</f>
-        <v>0.74017696877011452</v>
+        <v>0.85462636694652372</v>
       </c>
       <c r="J12">
         <f ca="1">Distances!J12/80</f>
-        <v>0.71750731545400304</v>
+        <v>0.20919878077761656</v>
       </c>
       <c r="K12">
         <f ca="1">Distances!K12/80</f>
-        <v>0.94445615154241103</v>
+        <v>1.9445501821094537</v>
       </c>
       <c r="L12">
         <f ca="1">Distances!L12/80</f>
@@ -3897,11 +3896,11 @@
       </c>
       <c r="M12">
         <f ca="1">Distances!M12/80</f>
-        <v>1.641364032924137</v>
+        <v>1.5801260419968337</v>
       </c>
       <c r="N12">
         <f ca="1">Distances!N12/80</f>
-        <v>1.13321174569794</v>
+        <v>0.3206096262204442</v>
       </c>
       <c r="O12">
         <f>Distances!O12/80</f>
@@ -3916,54 +3915,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <f ca="1">Distances!A13/80</f>
-        <v>0.99790081470241709</v>
+        <v>1.458053419047618</v>
       </c>
       <c r="B13">
         <f ca="1">Distances!B13/80</f>
-        <v>0.4031511289033104</v>
+        <v>1.2224210885212572</v>
       </c>
       <c r="C13">
         <f ca="1">Distances!C13/80</f>
-        <v>1.5970302302186912</v>
+        <v>2.1425159789995623</v>
       </c>
       <c r="D13">
         <f ca="1">Distances!D13/80</f>
-        <v>2.4105779407749788</v>
+        <v>1.6690325977313076</v>
       </c>
       <c r="E13">
         <f ca="1">Distances!E13/80</f>
-        <v>0.33251601609101195</v>
+        <v>2.8446376353054292</v>
       </c>
       <c r="F13">
         <f ca="1">Distances!F13/80</f>
-        <v>1.8449507761924671</v>
+        <v>1.0700523020075294</v>
       </c>
       <c r="G13">
         <f ca="1">Distances!G13/80</f>
-        <v>2.5648984053839463</v>
+        <v>1.9201158520223172</v>
       </c>
       <c r="H13">
         <f ca="1">Distances!H13/80</f>
-        <v>0.62119738779136502</v>
+        <v>2.1497081942455494</v>
       </c>
       <c r="I13">
         <f ca="1">Distances!I13/80</f>
-        <v>1.6872318275675124</v>
+        <v>1.6024582927207298</v>
       </c>
       <c r="J13">
         <f ca="1">Distances!J13/80</f>
-        <v>1.0531233643872113</v>
+        <v>1.6655661746910304</v>
       </c>
       <c r="K13">
         <f ca="1">Distances!K13/80</f>
-        <v>1.2700978849547284</v>
+        <v>2.1214138042385158</v>
       </c>
       <c r="L13">
         <f ca="1">Distances!L13/80</f>
-        <v>1.641364032924137</v>
+        <v>1.5801260419968337</v>
       </c>
       <c r="M13">
         <f ca="1">Distances!M13/80</f>
@@ -3971,7 +3970,7 @@
       </c>
       <c r="N13">
         <f ca="1">Distances!N13/80</f>
-        <v>0.99790081470241709</v>
+        <v>1.458053419047618</v>
       </c>
       <c r="O13">
         <f>Distances!O13/80</f>
@@ -3986,58 +3985,58 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>Distances!A14/80</f>
         <v>0</v>
       </c>
       <c r="B14">
         <f ca="1">Distances!B14/80</f>
-        <v>1.2622898324154117</v>
+        <v>0.78062868103877736</v>
       </c>
       <c r="C14">
         <f ca="1">Distances!C14/80</f>
-        <v>0.65065927910294397</v>
+        <v>1.2547817173828901</v>
       </c>
       <c r="D14">
         <f ca="1">Distances!D14/80</f>
-        <v>1.4221553667804445</v>
+        <v>0.74801012246417009</v>
       </c>
       <c r="E14">
         <f ca="1">Distances!E14/80</f>
-        <v>0.66556884819078477</v>
+        <v>1.4013396740268182</v>
       </c>
       <c r="F14">
         <f ca="1">Distances!F14/80</f>
-        <v>0.90749416435170893</v>
+        <v>0.70461692700604917</v>
       </c>
       <c r="G14">
         <f ca="1">Distances!G14/80</f>
-        <v>1.5764630132287945</v>
+        <v>0.85808780003504537</v>
       </c>
       <c r="H14">
         <f ca="1">Distances!H14/80</f>
-        <v>1.0052217014989184</v>
+        <v>1.1975767698093871</v>
       </c>
       <c r="I14">
         <f ca="1">Distances!I14/80</f>
-        <v>0.78992150831015484</v>
+        <v>0.54850800361316554</v>
       </c>
       <c r="J14">
         <f ca="1">Distances!J14/80</f>
-        <v>1.0377906093184419</v>
+        <v>0.2403586369706186</v>
       </c>
       <c r="K14">
         <f ca="1">Distances!K14/80</f>
-        <v>0.31176317981994589</v>
+        <v>1.6310517462871961</v>
       </c>
       <c r="L14">
         <f ca="1">Distances!L14/80</f>
-        <v>1.13321174569794</v>
+        <v>0.3206096262204442</v>
       </c>
       <c r="M14">
         <f ca="1">Distances!M14/80</f>
-        <v>0.99790081470241709</v>
+        <v>1.458053419047618</v>
       </c>
       <c r="N14">
         <f>Distances!N14/80</f>
@@ -4056,7 +4055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <f>Distances!A15/80</f>
         <v>0</v>
@@ -4126,7 +4125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>Distances!A16/80</f>
         <v>0</v>
@@ -4196,7 +4195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>Distances!A17/80</f>
         <v>0</v>

</xml_diff>